<commit_message>
docs: update user manual
</commit_message>
<xml_diff>
--- a/tests/NeoMedPRINT_test_5 KG.xlsx
+++ b/tests/NeoMedPRINT_test_5 KG.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10819" uniqueCount="3299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10819" uniqueCount="3296">
   <si>
     <t>Verwacht</t>
   </si>
@@ -10042,25 +10042,15 @@
     <t>10-200 nanogram/kg/min</t>
   </si>
   <si>
-    <t>6 uren</t>
-  </si>
-  <si>
-    <t>8 uren</t>
-  </si>
-  <si>
     <t>20 uren</t>
-  </si>
-  <si>
-    <t>22 uren</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -10170,7 +10160,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -10263,9 +10253,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -10663,13 +10650,13 @@
       <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomRight" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="5" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="16" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" style="16" customWidth="1"/>
     <col min="5" max="7" width="13" style="16" customWidth="1"/>
@@ -10685,7 +10672,7 @@
     <col min="17" max="17" width="22" style="16" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="25.28515625" style="16" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" style="39" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13" style="16" customWidth="1"/>
     <col min="22" max="22" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="31.140625" style="16" bestFit="1" customWidth="1"/>
@@ -10712,7 +10699,7 @@
   <sheetData>
     <row r="1" spans="1:51" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="3"/>
@@ -10721,7 +10708,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="25"/>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="40" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="3"/>
@@ -10734,9 +10721,9 @@
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
-      <c r="T1" s="38"/>
+      <c r="T1" s="37"/>
       <c r="U1" s="3"/>
-      <c r="V1" s="42" t="s">
+      <c r="V1" s="41" t="s">
         <v>54</v>
       </c>
       <c r="W1" s="3"/>
@@ -10829,7 +10816,7 @@
       <c r="S2" s="3" t="s">
         <v>3222</v>
       </c>
-      <c r="T2" s="38" t="s">
+      <c r="T2" s="37" t="s">
         <v>23</v>
       </c>
       <c r="U2" s="3" t="s">
@@ -10926,7 +10913,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>1</v>
       </c>
@@ -10957,7 +10944,7 @@
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
       <c r="S3" s="18"/>
-      <c r="T3" s="37">
+      <c r="T3" s="36">
         <v>0</v>
       </c>
       <c r="U3" s="18"/>
@@ -10983,134 +10970,133 @@
         <v>0</v>
       </c>
       <c r="AI3" s="16" t="b">
-        <f>AND(AJ3:AV3)</f>
+        <f t="shared" ref="AI3:AI26" si="0">AND(AJ3:AV3)</f>
         <v>1</v>
       </c>
       <c r="AJ3" s="16" t="b">
-        <f>I3=V3</f>
+        <f t="shared" ref="AJ3:AJ26" si="1">I3=V3</f>
         <v>1</v>
       </c>
       <c r="AK3" s="16" t="b">
-        <f>J3=W3</f>
+        <f t="shared" ref="AK3:AK26" si="2">J3=W3</f>
         <v>1</v>
       </c>
       <c r="AL3" s="16" t="b">
-        <f>K3=X3</f>
+        <f t="shared" ref="AL3:AL26" si="3">K3=X3</f>
         <v>1</v>
       </c>
       <c r="AM3" s="16" t="b">
-        <f>L3=Y3</f>
+        <f t="shared" ref="AM3:AM26" si="4">L3=Y3</f>
         <v>1</v>
       </c>
       <c r="AN3" s="16" t="b">
-        <f>M3=Z3</f>
+        <f t="shared" ref="AN3:AN26" si="5">M3=Z3</f>
         <v>1</v>
       </c>
       <c r="AO3" s="16" t="b">
-        <f>N3=AA3</f>
+        <f t="shared" ref="AO3:AO26" si="6">N3=AA3</f>
         <v>1</v>
       </c>
       <c r="AP3" s="16" t="b">
-        <f>O3=AB3</f>
+        <f t="shared" ref="AP3:AP26" si="7">O3=AB3</f>
         <v>1</v>
       </c>
       <c r="AQ3" s="16" t="b">
-        <f>P3=AC3</f>
+        <f t="shared" ref="AQ3:AQ26" si="8">P3=AC3</f>
         <v>1</v>
       </c>
       <c r="AR3" s="16" t="b">
-        <f>Q3=AD3</f>
+        <f t="shared" ref="AR3:AR26" si="9">Q3=AD3</f>
         <v>1</v>
       </c>
       <c r="AS3" s="16" t="b">
-        <f>R3=AE3</f>
+        <f t="shared" ref="AS3:AS26" si="10">R3=AE3</f>
         <v>1</v>
       </c>
       <c r="AT3" s="16" t="b">
-        <f>S3=AF3</f>
+        <f t="shared" ref="AT3:AT26" si="11">S3=AF3</f>
         <v>1</v>
       </c>
       <c r="AU3" s="16" t="b">
-        <f>T3=AG3</f>
+        <f t="shared" ref="AU3:AU26" si="12">T3=AG3</f>
         <v>1</v>
       </c>
       <c r="AV3" s="16" t="b">
-        <f>U3=AH3</f>
+        <f t="shared" ref="AV3:AV26" si="13">U3=AH3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
-        <f>A3+1</f>
+        <f t="shared" ref="A4:A26" si="14">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="6">
         <v>5</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="D4" s="17">
-        <v>240</v>
+        <v>0.8</v>
       </c>
       <c r="E4" s="17"/>
-      <c r="F4" s="17">
-        <v>24</v>
-      </c>
-      <c r="G4" s="17">
-        <v>4</v>
-      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
       <c r="H4" s="26" t="s">
         <v>3214</v>
       </c>
       <c r="I4" s="17">
-        <f>IF(B4="",1,B4)</f>
+        <f t="shared" ref="I4:I26" si="15">IF(B4="",1,B4)</f>
         <v>5</v>
       </c>
       <c r="J4" s="17" t="str">
-        <f>IF(C4="",1,C4)</f>
-        <v>doxapram</v>
-      </c>
-      <c r="K4" s="18">
-        <v>48</v>
-      </c>
-      <c r="L4" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4" s="17"/>
+        <f t="shared" ref="J4:J26" si="16">IF(C4="",1,C4)</f>
+        <v>adrenaline</v>
+      </c>
+      <c r="K4" s="17">
+        <v>0.8</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="17" t="str">
+        <f>IF(E4="","glucose 10%",E4)</f>
+        <v>glucose 10%</v>
+      </c>
       <c r="N4" s="17">
         <f>IF(F4="",12,F4)</f>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="O4" s="20">
         <f>IF(G4="",0.5,G4)</f>
-        <v>4</v>
-      </c>
-      <c r="P4" s="36">
-        <v>1.6</v>
+        <v>0.5</v>
+      </c>
+      <c r="P4" s="31">
+        <v>0.11</v>
       </c>
       <c r="Q4" s="18" t="s">
-        <v>3210</v>
+        <v>3207</v>
       </c>
       <c r="R4" s="18" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="S4" s="18" t="s">
-        <v>3295</v>
-      </c>
-      <c r="T4" s="37">
-        <f>K4/2</f>
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="T4" s="38">
+        <f>K4/0.1</f>
+        <v>8</v>
       </c>
       <c r="U4" s="34">
         <f>N4-T4</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V4" s="8">
         <v>5</v>
       </c>
       <c r="W4" s="9" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="X4" s="9"/>
       <c r="Y4" s="9"/>
@@ -11124,107 +11110,103 @@
       <c r="AG4" s="9"/>
       <c r="AH4" s="9"/>
       <c r="AI4" s="16" t="b">
-        <f>AND(AJ4:AV4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ4" s="16" t="b">
-        <f>I4=V4</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK4" s="16" t="b">
-        <f>J4=W4</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL4" s="16" t="b">
-        <f>K4=X4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM4" s="16" t="b">
-        <f>L4=Y4</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN4" s="16" t="b">
-        <f>M4=Z4</f>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="AO4" s="16" t="b">
-        <f>N4=AA4</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP4" s="16" t="b">
-        <f>O4=AB4</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ4" s="16" t="b">
-        <f>P4=AC4</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR4" s="16" t="b">
-        <f>Q4=AD4</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS4" s="16" t="b">
-        <f>R4=AE4</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT4" s="16" t="b">
-        <f>S4=AF4</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU4" s="16" t="b">
-        <f>T4=AG4</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV4" s="16" t="b">
-        <f>U4=AH4</f>
-        <v>1</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="AW4" s="16" t="s">
-        <v>3236</v>
+        <v>3226</v>
       </c>
       <c r="AX4" s="16" t="s">
-        <v>3275</v>
+        <v>3269</v>
       </c>
       <c r="AY4" s="16" t="s">
-        <v>3235</v>
+        <v>3225</v>
       </c>
     </row>
     <row r="5" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
-        <f>A4+1</f>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="B5" s="6">
         <v>5</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>41</v>
+        <v>3293</v>
       </c>
       <c r="D5" s="17">
-        <v>240</v>
+        <v>0.48</v>
       </c>
       <c r="E5" s="17"/>
-      <c r="F5" s="17">
-        <v>24</v>
-      </c>
-      <c r="G5" s="17">
-        <v>4</v>
-      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
       <c r="H5" s="26" t="s">
         <v>3214</v>
       </c>
       <c r="I5" s="17">
-        <f>IF(B5="",1,B5)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J5" s="17" t="str">
-        <f>IF(C5="",1,C5)</f>
-        <v>esmolol</v>
+        <f t="shared" si="16"/>
+        <v>alprostadil</v>
       </c>
       <c r="K5" s="17">
-        <v>240</v>
-      </c>
-      <c r="L5" s="18" t="s">
+        <v>0.24</v>
+      </c>
+      <c r="L5" s="17" t="s">
         <v>33</v>
       </c>
       <c r="M5" s="17" t="str">
@@ -11232,37 +11214,38 @@
         <v>glucose 10%</v>
       </c>
       <c r="N5" s="17">
-        <v>24</v>
+        <f>IF(F5="",12,F5)</f>
+        <v>12</v>
       </c>
       <c r="O5" s="20">
         <f>IF(G5="",0.5,G5)</f>
-        <v>4</v>
-      </c>
-      <c r="P5" s="32">
-        <v>0.13300000000000001</v>
+        <v>0.5</v>
+      </c>
+      <c r="P5" s="31">
+        <v>33</v>
       </c>
       <c r="Q5" s="18" t="s">
-        <v>3211</v>
+        <v>3208</v>
       </c>
       <c r="R5" s="18" t="s">
-        <v>63</v>
+        <v>3294</v>
       </c>
       <c r="S5" s="18" t="s">
-        <v>3295</v>
-      </c>
-      <c r="T5" s="37">
-        <f>K5/10</f>
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="T5" s="36">
+        <f>K5/0.5</f>
+        <v>0.48</v>
       </c>
       <c r="U5" s="34">
         <f>N5-T5</f>
-        <v>0</v>
+        <v>11.52</v>
       </c>
       <c r="V5" s="8">
         <v>5</v>
       </c>
       <c r="W5" s="9" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="X5" s="9"/>
       <c r="Y5" s="9"/>
@@ -11276,105 +11259,101 @@
       <c r="AG5" s="9"/>
       <c r="AH5" s="9"/>
       <c r="AI5" s="16" t="b">
-        <f>AND(AJ5:AV5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ5" s="16" t="b">
-        <f>I5=V5</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK5" s="16" t="b">
-        <f>J5=W5</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="AL5" s="16" t="b">
-        <f>K5=X5</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM5" s="16" t="b">
-        <f>L5=Y5</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN5" s="16" t="b">
-        <f>M5=Z5</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AO5" s="16" t="b">
-        <f>N5=AA5</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP5" s="16" t="b">
-        <f>O5=AB5</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ5" s="16" t="b">
-        <f>P5=AC5</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR5" s="16" t="b">
-        <f>Q5=AD5</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS5" s="16" t="b">
-        <f>R5=AE5</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT5" s="16" t="b">
-        <f>S5=AF5</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU5" s="16" t="b">
-        <f>T5=AG5</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV5" s="16" t="b">
-        <f>U5=AH5</f>
-        <v>1</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="AW5" s="16" t="s">
-        <v>3240</v>
+        <v>3228</v>
       </c>
       <c r="AX5" s="16" t="s">
-        <v>3277</v>
+        <v>3270</v>
       </c>
       <c r="AY5" s="16" t="s">
-        <v>3239</v>
+        <v>3227</v>
       </c>
     </row>
     <row r="6" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
-        <f>A5+1</f>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="B6" s="6">
         <v>5</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>3293</v>
+        <v>31</v>
       </c>
       <c r="D6" s="17">
-        <v>1.44</v>
+        <v>120</v>
       </c>
       <c r="E6" s="17"/>
-      <c r="F6" s="17">
-        <v>24</v>
-      </c>
-      <c r="G6" s="17">
-        <v>3</v>
-      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
       <c r="H6" s="26" t="s">
         <v>3214</v>
       </c>
       <c r="I6" s="17">
-        <f>IF(B6="",1,B6)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J6" s="17" t="str">
-        <f>IF(C6="",1,C6)</f>
-        <v>alprostadil</v>
+        <f t="shared" si="16"/>
+        <v>amiodarone</v>
       </c>
       <c r="K6" s="17">
-        <v>0.48</v>
+        <v>120</v>
       </c>
       <c r="L6" s="17" t="s">
         <v>33</v>
@@ -11385,31 +11364,31 @@
       </c>
       <c r="N6" s="17">
         <f>IF(F6="",12,F6)</f>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="O6" s="20">
         <f>IF(G6="",0.5,G6)</f>
-        <v>3</v>
-      </c>
-      <c r="P6" s="32">
-        <v>200</v>
+        <v>0.5</v>
+      </c>
+      <c r="P6" s="31">
+        <v>17</v>
       </c>
       <c r="Q6" s="18" t="s">
-        <v>3208</v>
+        <v>3207</v>
       </c>
       <c r="R6" s="18" t="s">
-        <v>3294</v>
+        <v>55</v>
       </c>
       <c r="S6" s="18" t="s">
-        <v>3296</v>
-      </c>
-      <c r="T6" s="37">
-        <f>K6/0.5</f>
-        <v>0.96</v>
+        <v>35</v>
+      </c>
+      <c r="T6" s="36">
+        <f>K6/50</f>
+        <v>2.4</v>
       </c>
       <c r="U6" s="34">
         <f>N6-T6</f>
-        <v>23.04</v>
+        <v>9.6</v>
       </c>
       <c r="V6" s="8">
         <v>5</v>
@@ -11429,59 +11408,59 @@
       <c r="AG6" s="9"/>
       <c r="AH6" s="9"/>
       <c r="AI6" s="16" t="b">
-        <f>AND(AJ6:AV6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ6" s="16" t="b">
-        <f>I6=V6</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK6" s="16" t="b">
-        <f>J6=W6</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="AL6" s="16" t="b">
-        <f>K6=X6</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM6" s="16" t="b">
-        <f>L6=Y6</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN6" s="16" t="b">
-        <f>M6=Z6</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AO6" s="16" t="b">
-        <f>N6=AA6</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP6" s="16" t="b">
-        <f>O6=AB6</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ6" s="16" t="b">
-        <f>P6=AC6</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR6" s="16" t="b">
-        <f>Q6=AD6</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS6" s="16" t="b">
-        <f>R6=AE6</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT6" s="16" t="b">
-        <f>S6=AF6</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU6" s="16" t="b">
-        <f>T6=AG6</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV6" s="16" t="b">
-        <f>U6=AH6</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AW6" s="16" t="s">
@@ -11496,79 +11475,74 @@
     </row>
     <row r="7" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
-        <f>A6+1</f>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="B7" s="6">
         <v>5</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="D7" s="17">
-        <v>360</v>
+        <v>5</v>
       </c>
       <c r="E7" s="17"/>
-      <c r="F7" s="17">
-        <v>24</v>
-      </c>
-      <c r="G7" s="17">
-        <v>3</v>
-      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="26" t="s">
         <v>3214</v>
       </c>
       <c r="I7" s="17">
-        <f>IF(B7="",1,B7)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J7" s="17" t="str">
-        <f>IF(C7="",1,C7)</f>
-        <v>labetalol</v>
+        <f t="shared" si="16"/>
+        <v>bupivacaine EPIDURAAL</v>
       </c>
       <c r="K7" s="17">
-        <v>120</v>
+        <f>IF(D7="",1,D7)</f>
+        <v>5</v>
       </c>
       <c r="L7" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" s="17" t="str">
-        <f>IF(E7="","glucose 10%",E7)</f>
-        <v>glucose 10%</v>
+        <v>56</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="N7" s="17">
-        <f>IF(F7="",12,F7)</f>
+        <f>IF(F7="",24,F7)</f>
         <v>24</v>
       </c>
       <c r="O7" s="20">
-        <f>IF(G7="",0.5,G7)</f>
-        <v>3</v>
-      </c>
-      <c r="P7" s="32">
-        <v>3</v>
+        <f>IF(G7="",1,G7)</f>
+        <v>1</v>
+      </c>
+      <c r="P7" s="31">
+        <v>1</v>
       </c>
       <c r="Q7" s="18" t="s">
-        <v>3210</v>
+        <v>3291</v>
       </c>
       <c r="R7" s="18" t="s">
-        <v>75</v>
+        <v>3292</v>
       </c>
       <c r="S7" s="18" t="s">
-        <v>3296</v>
-      </c>
-      <c r="T7" s="37">
-        <f>K7/5</f>
-        <v>24</v>
-      </c>
-      <c r="U7" s="34">
-        <f>N7-T7</f>
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="T7" s="36">
+        <f>K7/1</f>
+        <v>5</v>
+      </c>
+      <c r="U7" s="18">
+        <v>19</v>
       </c>
       <c r="V7" s="8">
         <v>5</v>
       </c>
       <c r="W7" s="9" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="X7" s="9"/>
       <c r="Y7" s="9"/>
@@ -11582,143 +11556,141 @@
       <c r="AG7" s="9"/>
       <c r="AH7" s="9"/>
       <c r="AI7" s="16" t="b">
-        <f>AND(AJ7:AV7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ7" s="16" t="b">
-        <f>I7=V7</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK7" s="16" t="b">
-        <f>J7=W7</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL7" s="16" t="b">
-        <f>K7=X7</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM7" s="16" t="b">
-        <f>L7=Y7</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN7" s="16" t="b">
-        <f>M7=Z7</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AO7" s="16" t="b">
-        <f>N7=AA7</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP7" s="16" t="b">
-        <f>O7=AB7</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ7" s="16" t="b">
-        <f>P7=AC7</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR7" s="16" t="b">
-        <f>Q7=AD7</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS7" s="16" t="b">
-        <f>R7=AE7</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT7" s="16" t="b">
-        <f>S7=AF7</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU7" s="16" t="b">
-        <f>T7=AG7</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV7" s="16" t="b">
-        <f>U7=AH7</f>
-        <v>1</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="AW7" s="16" t="s">
-        <v>3248</v>
+        <v>3266</v>
       </c>
       <c r="AX7" s="16" t="s">
-        <v>3281</v>
+        <v>3271</v>
       </c>
       <c r="AY7" s="16" t="s">
-        <v>3247</v>
+        <v>3265</v>
       </c>
     </row>
     <row r="8" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
-        <f>A7+1</f>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="B8" s="6">
         <v>5</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D8" s="17">
-        <v>0.28799999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="E8" s="17"/>
-      <c r="F8" s="17">
-        <v>24</v>
-      </c>
-      <c r="G8" s="17">
-        <v>1.2</v>
-      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
       <c r="H8" s="26" t="s">
         <v>3214</v>
       </c>
       <c r="I8" s="17">
-        <f>IF(B8="",1,B8)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J8" s="17" t="str">
-        <f>IF(C8="",1,C8)</f>
-        <v>epoprostenol</v>
+        <f t="shared" si="16"/>
+        <v>clonidine</v>
       </c>
       <c r="K8" s="17">
-        <v>0.24</v>
+        <v>0.3</v>
       </c>
       <c r="L8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="M8" s="17"/>
+      <c r="M8" s="17" t="s">
+        <v>57</v>
+      </c>
       <c r="N8" s="17">
         <f>IF(F8="",12,F8)</f>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="O8" s="20">
-        <f>IF(G8="",0.5,G8)</f>
-        <v>1.2</v>
+        <f t="shared" ref="O8:O17" si="17">IF(G8="",0.5,G8)</f>
+        <v>0.5</v>
       </c>
       <c r="P8" s="31">
-        <v>40</v>
+        <v>2.5</v>
       </c>
       <c r="Q8" s="18" t="s">
-        <v>3208</v>
+        <v>3209</v>
       </c>
       <c r="R8" s="18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="S8" s="18" t="s">
-        <v>3297</v>
-      </c>
-      <c r="T8" s="37">
-        <f>K8/0.01</f>
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="T8" s="36">
+        <f>K8/0.15</f>
+        <v>2</v>
       </c>
       <c r="U8" s="34">
-        <f>N8-T8</f>
-        <v>0</v>
+        <f t="shared" ref="U8:U25" si="18">N8-T8</f>
+        <v>10</v>
       </c>
       <c r="V8" s="8">
         <v>5</v>
       </c>
       <c r="W8" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="X8" s="9"/>
       <c r="Y8" s="9"/>
@@ -11732,146 +11704,139 @@
       <c r="AG8" s="9"/>
       <c r="AH8" s="9"/>
       <c r="AI8" s="16" t="b">
-        <f>AND(AJ8:AV8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ8" s="16" t="b">
-        <f>I8=V8</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK8" s="16" t="b">
-        <f>J8=W8</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL8" s="16" t="b">
-        <f>K8=X8</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM8" s="16" t="b">
-        <f>L8=Y8</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN8" s="16" t="b">
-        <f>M8=Z8</f>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="AO8" s="16" t="b">
-        <f>N8=AA8</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP8" s="16" t="b">
-        <f>O8=AB8</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ8" s="16" t="b">
-        <f>P8=AC8</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR8" s="16" t="b">
-        <f>Q8=AD8</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS8" s="16" t="b">
-        <f>R8=AE8</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT8" s="16" t="b">
-        <f>S8=AF8</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU8" s="16" t="b">
-        <f>T8=AG8</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV8" s="16" t="b">
-        <f>U8=AH8</f>
-        <v>1</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="AW8" s="16" t="s">
-        <v>3238</v>
+        <v>3230</v>
       </c>
       <c r="AX8" s="16" t="s">
-        <v>3276</v>
+        <v>3272</v>
       </c>
       <c r="AY8" s="16" t="s">
-        <v>3237</v>
+        <v>3229</v>
       </c>
     </row>
     <row r="9" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
-        <f>A8+1</f>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="B9" s="6">
         <v>5</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D9" s="17">
-        <v>264</v>
+        <v>144</v>
       </c>
       <c r="E9" s="17"/>
-      <c r="F9" s="17">
-        <v>24</v>
-      </c>
-      <c r="G9" s="17">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
       <c r="H9" s="26" t="s">
         <v>3214</v>
       </c>
       <c r="I9" s="17">
-        <f>IF(B9="",1,B9)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J9" s="17" t="str">
-        <f>IF(C9="",1,C9)</f>
-        <v>rocuronium</v>
+        <f t="shared" si="16"/>
+        <v>dobutamine</v>
       </c>
       <c r="K9" s="17">
-        <v>240</v>
+        <v>150</v>
       </c>
       <c r="L9" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="M9" s="17" t="str">
-        <f>IF(E9="","glucose 10%",E9)</f>
-        <v>glucose 10%</v>
-      </c>
+      <c r="M9" s="17"/>
       <c r="N9" s="17">
         <f>IF(F9="",12,F9)</f>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="O9" s="20">
-        <f>IF(G9="",0.5,G9)</f>
-        <v>1.1000000000000001</v>
+        <f t="shared" si="17"/>
+        <v>0.5</v>
       </c>
       <c r="P9" s="31">
-        <v>2.2000000000000002</v>
+        <v>21</v>
       </c>
       <c r="Q9" s="18" t="s">
-        <v>3210</v>
+        <v>3207</v>
       </c>
       <c r="R9" s="18" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="S9" s="18" t="s">
-        <v>3298</v>
-      </c>
-      <c r="T9" s="37">
-        <f>K9/10</f>
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="T9" s="36">
+        <f>K9/12.5</f>
+        <v>12</v>
       </c>
       <c r="U9" s="34">
-        <f>N9-T9</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="V9" s="8">
         <v>5</v>
       </c>
       <c r="W9" s="9" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="X9" s="9"/>
       <c r="Y9" s="9"/>
@@ -11885,141 +11850,143 @@
       <c r="AG9" s="9"/>
       <c r="AH9" s="9"/>
       <c r="AI9" s="16" t="b">
-        <f>AND(AJ9:AV9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ9" s="16" t="b">
-        <f>I9=V9</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK9" s="16" t="b">
-        <f>J9=W9</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL9" s="16" t="b">
-        <f>K9=X9</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM9" s="16" t="b">
-        <f>L9=Y9</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN9" s="16" t="b">
-        <f>M9=Z9</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="AO9" s="16" t="b">
-        <f>N9=AA9</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP9" s="16" t="b">
-        <f>O9=AB9</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ9" s="16" t="b">
-        <f>P9=AC9</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR9" s="16" t="b">
-        <f>Q9=AD9</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS9" s="16" t="b">
-        <f>R9=AE9</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT9" s="16" t="b">
-        <f>S9=AF9</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU9" s="16" t="b">
-        <f>T9=AG9</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV9" s="16" t="b">
-        <f>U9=AH9</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AW9" s="16" t="s">
-        <v>3264</v>
+        <v>3232</v>
       </c>
       <c r="AX9" s="16" t="s">
-        <v>3289</v>
+        <v>3273</v>
       </c>
       <c r="AY9" s="16" t="s">
-        <v>3263</v>
+        <v>3231</v>
       </c>
     </row>
     <row r="10" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
-        <f>A9+1</f>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B10" s="6">
         <v>5</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="17">
-        <v>14.4</v>
+        <v>38</v>
+      </c>
+      <c r="D10" s="22">
+        <v>144</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
-      <c r="G10" s="17">
-        <v>0.6</v>
-      </c>
+      <c r="G10" s="17"/>
       <c r="H10" s="26" t="s">
         <v>3214</v>
       </c>
       <c r="I10" s="17">
-        <f>IF(B10="",1,B10)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J10" s="17" t="str">
-        <f>IF(C10="",1,C10)</f>
-        <v>nicardipine</v>
+        <f t="shared" si="16"/>
+        <v>dopamine</v>
       </c>
       <c r="K10" s="17">
-        <v>12</v>
+        <f>IF(D10="",1.44,D10)</f>
+        <v>144</v>
       </c>
       <c r="L10" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="17"/>
+      <c r="M10" s="17" t="str">
+        <f>IF(E10="","glucose 10%",E10)</f>
+        <v>glucose 10%</v>
+      </c>
       <c r="N10" s="17">
         <f>IF(F10="",12,F10)</f>
         <v>12</v>
       </c>
       <c r="O10" s="20">
-        <f>IF(G10="",0.5,G10)</f>
-        <v>0.6</v>
-      </c>
-      <c r="P10" s="32">
-        <v>2</v>
+        <f t="shared" si="17"/>
+        <v>0.5</v>
+      </c>
+      <c r="P10" s="31">
+        <v>20</v>
       </c>
       <c r="Q10" s="18" t="s">
         <v>3207</v>
       </c>
       <c r="R10" s="18" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="S10" s="18" t="s">
-        <v>3297</v>
-      </c>
-      <c r="T10" s="37">
-        <f>K10/1</f>
-        <v>12</v>
+        <v>35</v>
+      </c>
+      <c r="T10" s="36">
+        <f>K10/40</f>
+        <v>3.6</v>
       </c>
       <c r="U10" s="34">
-        <f>N10-T10</f>
-        <v>0</v>
+        <f t="shared" si="18"/>
+        <v>8.4</v>
       </c>
       <c r="V10" s="8">
         <v>5</v>
       </c>
       <c r="W10" s="9" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="X10" s="9"/>
       <c r="Y10" s="9"/>
@@ -12033,103 +12000,101 @@
       <c r="AG10" s="9"/>
       <c r="AH10" s="9"/>
       <c r="AI10" s="16" t="b">
-        <f>AND(AJ10:AV10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ10" s="16" t="b">
-        <f>I10=V10</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK10" s="16" t="b">
-        <f>J10=W10</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL10" s="16" t="b">
-        <f>K10=X10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM10" s="16" t="b">
-        <f>L10=Y10</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN10" s="16" t="b">
-        <f>M10=Z10</f>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="AO10" s="16" t="b">
-        <f>N10=AA10</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP10" s="16" t="b">
-        <f>O10=AB10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ10" s="16" t="b">
-        <f>P10=AC10</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR10" s="16" t="b">
-        <f>Q10=AD10</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS10" s="16" t="b">
-        <f>R10=AE10</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT10" s="16" t="b">
-        <f>S10=AF10</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU10" s="16" t="b">
-        <f>T10=AG10</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV10" s="16" t="b">
-        <f>U10=AH10</f>
-        <v>1</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="AW10" s="16" t="s">
-        <v>3258</v>
+        <v>3234</v>
       </c>
       <c r="AX10" s="16" t="s">
-        <v>3286</v>
+        <v>3274</v>
       </c>
       <c r="AY10" s="16" t="s">
-        <v>3257</v>
+        <v>3233</v>
       </c>
     </row>
     <row r="11" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
-        <f>A10+1</f>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="B11" s="6">
         <v>5</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D11" s="17">
-        <v>14.4</v>
+        <v>48</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
-      <c r="G11" s="17">
-        <v>0.6</v>
-      </c>
+      <c r="G11" s="17"/>
       <c r="H11" s="26" t="s">
         <v>3214</v>
       </c>
       <c r="I11" s="17">
-        <f>IF(B11="",1,B11)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J11" s="17" t="str">
-        <f>IF(C11="",1,C11)</f>
-        <v>noradrenaline</v>
-      </c>
-      <c r="K11" s="17">
-        <v>12</v>
+        <f t="shared" si="16"/>
+        <v>doxapram</v>
+      </c>
+      <c r="K11" s="18">
+        <v>24</v>
       </c>
       <c r="L11" s="18" t="s">
         <v>33</v>
@@ -12140,34 +12105,34 @@
         <v>12</v>
       </c>
       <c r="O11" s="20">
-        <f>IF(G11="",0.5,G11)</f>
-        <v>0.6</v>
-      </c>
-      <c r="P11" s="32">
-        <v>2</v>
+        <f t="shared" si="17"/>
+        <v>0.5</v>
+      </c>
+      <c r="P11" s="31">
+        <v>0.2</v>
       </c>
       <c r="Q11" s="18" t="s">
-        <v>3207</v>
+        <v>3210</v>
       </c>
       <c r="R11" s="18" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="S11" s="18" t="s">
-        <v>3297</v>
-      </c>
-      <c r="T11" s="37">
-        <f>K11/1</f>
+        <v>35</v>
+      </c>
+      <c r="T11" s="36">
+        <f>K11/2</f>
         <v>12</v>
       </c>
       <c r="U11" s="34">
-        <f>N11-T11</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="V11" s="8">
         <v>5</v>
       </c>
       <c r="W11" s="9" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
@@ -12181,84 +12146,84 @@
       <c r="AG11" s="9"/>
       <c r="AH11" s="9"/>
       <c r="AI11" s="16" t="b">
-        <f>AND(AJ11:AV11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ11" s="16" t="b">
-        <f>I11=V11</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK11" s="16" t="b">
-        <f>J11=W11</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL11" s="16" t="b">
-        <f>K11=X11</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM11" s="16" t="b">
-        <f>L11=Y11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN11" s="16" t="b">
-        <f>M11=Z11</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AO11" s="16" t="b">
-        <f>N11=AA11</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP11" s="16" t="b">
-        <f>O11=AB11</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ11" s="16" t="b">
-        <f>P11=AC11</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR11" s="16" t="b">
-        <f>Q11=AD11</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS11" s="16" t="b">
-        <f>R11=AE11</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT11" s="16" t="b">
-        <f>S11=AF11</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU11" s="16" t="b">
-        <f>T11=AG11</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV11" s="16" t="b">
-        <f>U11=AH11</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AW11" s="16" t="s">
-        <v>3262</v>
+        <v>3236</v>
       </c>
       <c r="AX11" s="16" t="s">
-        <v>3288</v>
+        <v>3275</v>
       </c>
       <c r="AY11" s="16" t="s">
-        <v>3261</v>
+        <v>3235</v>
       </c>
     </row>
     <row r="12" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
-        <f>A11+1</f>
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
       <c r="B12" s="6">
         <v>5</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="D12" s="17">
-        <v>0.8</v>
+        <v>0.24</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
@@ -12267,56 +12232,53 @@
         <v>3214</v>
       </c>
       <c r="I12" s="17">
-        <f>IF(B12="",1,B12)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J12" s="17" t="str">
-        <f>IF(C12="",1,C12)</f>
-        <v>adrenaline</v>
+        <f t="shared" si="16"/>
+        <v>epoprostenol</v>
       </c>
       <c r="K12" s="17">
-        <v>0.8</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="M12" s="17" t="str">
-        <f>IF(E12="","glucose 10%",E12)</f>
-        <v>glucose 10%</v>
-      </c>
+        <v>0.12</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" s="17"/>
       <c r="N12" s="17">
         <f>IF(F12="",12,F12)</f>
         <v>12</v>
       </c>
       <c r="O12" s="20">
-        <f>IF(G12="",0.5,G12)</f>
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="P12" s="33">
-        <v>0.11</v>
+      <c r="P12" s="31">
+        <v>17</v>
       </c>
       <c r="Q12" s="18" t="s">
-        <v>3207</v>
+        <v>3208</v>
       </c>
       <c r="R12" s="18" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="S12" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="T12" s="39">
-        <f>K12/0.1</f>
-        <v>8</v>
+      <c r="T12" s="36">
+        <f>K12/0.01</f>
+        <v>12</v>
       </c>
       <c r="U12" s="34">
-        <f>N12-T12</f>
-        <v>4</v>
+        <f t="shared" si="18"/>
+        <v>0</v>
       </c>
       <c r="V12" s="8">
         <v>5</v>
       </c>
       <c r="W12" s="9" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="X12" s="9"/>
       <c r="Y12" s="9"/>
@@ -12330,84 +12292,84 @@
       <c r="AG12" s="9"/>
       <c r="AH12" s="9"/>
       <c r="AI12" s="16" t="b">
-        <f>AND(AJ12:AV12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ12" s="16" t="b">
-        <f>I12=V12</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK12" s="16" t="b">
-        <f>J12=W12</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL12" s="16" t="b">
-        <f>K12=X12</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM12" s="16" t="b">
-        <f>L12=Y12</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN12" s="16" t="b">
-        <f>M12=Z12</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="AO12" s="16" t="b">
-        <f>N12=AA12</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP12" s="16" t="b">
-        <f>O12=AB12</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ12" s="16" t="b">
-        <f>P12=AC12</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR12" s="16" t="b">
-        <f>Q12=AD12</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS12" s="16" t="b">
-        <f>R12=AE12</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT12" s="16" t="b">
-        <f>S12=AF12</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU12" s="16" t="b">
-        <f>T12=AG12</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV12" s="16" t="b">
-        <f>U12=AH12</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="AW12" s="16" t="s">
-        <v>3226</v>
+        <v>3238</v>
       </c>
       <c r="AX12" s="16" t="s">
-        <v>3269</v>
+        <v>3276</v>
       </c>
       <c r="AY12" s="16" t="s">
-        <v>3225</v>
+        <v>3237</v>
       </c>
     </row>
     <row r="13" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
-        <f>A12+1</f>
+        <f t="shared" si="14"/>
         <v>11</v>
       </c>
       <c r="B13" s="6">
         <v>5</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D13" s="17">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -12416,56 +12378,52 @@
         <v>3214</v>
       </c>
       <c r="I13" s="17">
-        <f>IF(B13="",1,B13)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J13" s="17" t="str">
-        <f>IF(C13="",1,C13)</f>
-        <v>amiodarone</v>
+        <f t="shared" si="16"/>
+        <v>esmolol</v>
       </c>
       <c r="K13" s="17">
         <v>120</v>
       </c>
-      <c r="L13" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="M13" s="17" t="str">
-        <f>IF(E13="","glucose 10%",E13)</f>
-        <v>glucose 10%</v>
-      </c>
+      <c r="L13" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" s="17"/>
       <c r="N13" s="17">
-        <f>IF(F13="",12,F13)</f>
         <v>12</v>
       </c>
       <c r="O13" s="20">
-        <f>IF(G13="",0.5,G13)</f>
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="P13" s="32">
-        <v>17</v>
+      <c r="P13" s="31">
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="Q13" s="18" t="s">
-        <v>3207</v>
+        <v>3211</v>
       </c>
       <c r="R13" s="18" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="S13" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="T13" s="37">
-        <f>K13/50</f>
-        <v>2.4</v>
+      <c r="T13" s="36">
+        <f>K13/10</f>
+        <v>12</v>
       </c>
       <c r="U13" s="34">
-        <f>N13-T13</f>
-        <v>9.6</v>
+        <f t="shared" si="18"/>
+        <v>0</v>
       </c>
       <c r="V13" s="8">
         <v>5</v>
       </c>
       <c r="W13" s="9" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="X13" s="9"/>
       <c r="Y13" s="9"/>
@@ -12479,84 +12437,84 @@
       <c r="AG13" s="9"/>
       <c r="AH13" s="9"/>
       <c r="AI13" s="16" t="b">
-        <f>AND(AJ13:AV13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ13" s="16" t="b">
-        <f>I13=V13</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK13" s="16" t="b">
-        <f>J13=W13</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL13" s="16" t="b">
-        <f>K13=X13</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM13" s="16" t="b">
-        <f>L13=Y13</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN13" s="16" t="b">
-        <f>M13=Z13</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="AO13" s="16" t="b">
-        <f>N13=AA13</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP13" s="16" t="b">
-        <f>O13=AB13</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ13" s="16" t="b">
-        <f>P13=AC13</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR13" s="16" t="b">
-        <f>Q13=AD13</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS13" s="16" t="b">
-        <f>R13=AE13</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT13" s="16" t="b">
-        <f>S13=AF13</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU13" s="16" t="b">
-        <f>T13=AG13</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV13" s="16" t="b">
-        <f>U13=AH13</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="AW13" s="16" t="s">
-        <v>3228</v>
+        <v>3240</v>
       </c>
       <c r="AX13" s="16" t="s">
-        <v>3270</v>
+        <v>3277</v>
       </c>
       <c r="AY13" s="16" t="s">
-        <v>3227</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="14" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
-        <f>A13+1</f>
+        <f t="shared" si="14"/>
         <v>12</v>
       </c>
       <c r="B14" s="6">
         <v>5</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D14" s="17">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
@@ -12565,55 +12523,57 @@
         <v>3214</v>
       </c>
       <c r="I14" s="17">
-        <f>IF(B14="",1,B14)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J14" s="17" t="str">
-        <f>IF(C14="",1,C14)</f>
-        <v>bupivacaine EPIDURAAL</v>
+        <f t="shared" si="16"/>
+        <v>furosemide</v>
       </c>
       <c r="K14" s="17">
-        <f>IF(D14="",1,D14)</f>
-        <v>5</v>
+        <f>IF(D14="",1.2,D14)</f>
+        <v>20</v>
       </c>
       <c r="L14" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="M14" s="17" t="s">
-        <v>57</v>
+        <v>33</v>
+      </c>
+      <c r="M14" s="17" t="str">
+        <f>IF(E14="","glucose 10%",E14)</f>
+        <v>glucose 10%</v>
       </c>
       <c r="N14" s="17">
-        <f>IF(F14="",24,F14)</f>
-        <v>24</v>
+        <f>IF(F14="",12,F14)</f>
+        <v>12</v>
       </c>
       <c r="O14" s="20">
-        <f>IF(G14="",1,G14)</f>
-        <v>1</v>
-      </c>
-      <c r="P14" s="32">
-        <v>1</v>
+        <f t="shared" si="17"/>
+        <v>0.5</v>
+      </c>
+      <c r="P14" s="31">
+        <v>4</v>
       </c>
       <c r="Q14" s="18" t="s">
-        <v>3291</v>
+        <v>3212</v>
       </c>
       <c r="R14" s="18" t="s">
-        <v>3292</v>
+        <v>65</v>
       </c>
       <c r="S14" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="T14" s="37">
-        <f>K14/1</f>
-        <v>5</v>
-      </c>
-      <c r="U14" s="18">
-        <v>19</v>
+      <c r="T14" s="36">
+        <f>K14/10</f>
+        <v>2</v>
+      </c>
+      <c r="U14" s="34">
+        <f t="shared" si="18"/>
+        <v>10</v>
       </c>
       <c r="V14" s="8">
         <v>5</v>
       </c>
       <c r="W14" s="9" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="X14" s="9"/>
       <c r="Y14" s="9"/>
@@ -12627,84 +12587,84 @@
       <c r="AG14" s="9"/>
       <c r="AH14" s="9"/>
       <c r="AI14" s="16" t="b">
-        <f>AND(AJ14:AV14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ14" s="16" t="b">
-        <f>I14=V14</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK14" s="16" t="b">
-        <f>J14=W14</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL14" s="16" t="b">
-        <f>K14=X14</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM14" s="16" t="b">
-        <f>L14=Y14</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN14" s="16" t="b">
-        <f>M14=Z14</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AO14" s="16" t="b">
-        <f>N14=AA14</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP14" s="16" t="b">
-        <f>O14=AB14</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ14" s="16" t="b">
-        <f>P14=AC14</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR14" s="16" t="b">
-        <f>Q14=AD14</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS14" s="16" t="b">
-        <f>R14=AE14</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT14" s="16" t="b">
-        <f>S14=AF14</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU14" s="16" t="b">
-        <f>T14=AG14</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV14" s="16" t="b">
-        <f>U14=AH14</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AW14" s="16" t="s">
-        <v>3266</v>
+        <v>3242</v>
       </c>
       <c r="AX14" s="16" t="s">
-        <v>3271</v>
+        <v>3278</v>
       </c>
       <c r="AY14" s="16" t="s">
-        <v>3265</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="15" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
-        <f>A14+1</f>
+        <f t="shared" si="14"/>
         <v>13</v>
       </c>
       <c r="B15" s="6">
         <v>5</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D15" s="17">
-        <v>0.3</v>
+        <v>12</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
@@ -12713,55 +12673,54 @@
         <v>3214</v>
       </c>
       <c r="I15" s="17">
-        <f>IF(B15="",1,B15)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J15" s="17" t="str">
-        <f>IF(C15="",1,C15)</f>
-        <v>clonidine</v>
+        <f t="shared" si="16"/>
+        <v>insuline</v>
       </c>
       <c r="K15" s="17">
-        <v>0.3</v>
+        <f>IF(D15="",0.24,D15)</f>
+        <v>12</v>
       </c>
       <c r="L15" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M15" s="17" t="s">
-        <v>57</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="M15" s="17"/>
       <c r="N15" s="17">
         <f>IF(F15="",12,F15)</f>
         <v>12</v>
       </c>
       <c r="O15" s="20">
-        <f>IF(G15="",0.5,G15)</f>
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="P15" s="36">
-        <v>2.5</v>
+      <c r="P15" s="31">
+        <v>0.1</v>
       </c>
       <c r="Q15" s="18" t="s">
-        <v>3209</v>
+        <v>3213</v>
       </c>
       <c r="R15" s="18" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="S15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="T15" s="37">
-        <f>K15/0.15</f>
-        <v>2</v>
+      <c r="T15" s="36">
+        <f>K15/1</f>
+        <v>12</v>
       </c>
       <c r="U15" s="34">
-        <f>N15-T15</f>
-        <v>10</v>
+        <f t="shared" si="18"/>
+        <v>0</v>
       </c>
       <c r="V15" s="8">
         <v>5</v>
       </c>
       <c r="W15" s="9" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="X15" s="9"/>
       <c r="Y15" s="9"/>
@@ -12775,84 +12734,84 @@
       <c r="AG15" s="9"/>
       <c r="AH15" s="9"/>
       <c r="AI15" s="16" t="b">
-        <f>AND(AJ15:AV15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ15" s="16" t="b">
-        <f>I15=V15</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK15" s="16" t="b">
-        <f>J15=W15</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL15" s="16" t="b">
-        <f>K15=X15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM15" s="16" t="b">
-        <f>L15=Y15</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN15" s="16" t="b">
-        <f>M15=Z15</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="AO15" s="16" t="b">
-        <f>N15=AA15</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP15" s="16" t="b">
-        <f>O15=AB15</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ15" s="16" t="b">
-        <f>P15=AC15</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR15" s="16" t="b">
-        <f>Q15=AD15</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS15" s="16" t="b">
-        <f>R15=AE15</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT15" s="16" t="b">
-        <f>S15=AF15</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU15" s="16" t="b">
-        <f>T15=AG15</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV15" s="16" t="b">
-        <f>U15=AH15</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="AW15" s="16" t="s">
-        <v>3230</v>
+        <v>3244</v>
       </c>
       <c r="AX15" s="16" t="s">
-        <v>3272</v>
+        <v>3279</v>
       </c>
       <c r="AY15" s="16" t="s">
-        <v>3229</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="16" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
-        <f>A15+1</f>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="B16" s="6">
         <v>5</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D16" s="17">
-        <v>144</v>
+        <v>10.8</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
@@ -12861,53 +12820,56 @@
         <v>3214</v>
       </c>
       <c r="I16" s="17">
-        <f>IF(B16="",1,B16)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J16" s="17" t="str">
-        <f>IF(C16="",1,C16)</f>
-        <v>dobutamine</v>
+        <f t="shared" si="16"/>
+        <v>isoprenaline</v>
       </c>
       <c r="K16" s="17">
-        <v>150</v>
+        <v>11</v>
       </c>
       <c r="L16" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="M16" s="17"/>
+      <c r="M16" s="17" t="str">
+        <f>IF(E16="","glucose 10%",E16)</f>
+        <v>glucose 10%</v>
+      </c>
       <c r="N16" s="17">
         <f>IF(F16="",12,F16)</f>
         <v>12</v>
       </c>
       <c r="O16" s="20">
-        <f>IF(G16="",0.5,G16)</f>
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="P16" s="36">
-        <v>21</v>
+      <c r="P16" s="31">
+        <v>1.5</v>
       </c>
       <c r="Q16" s="18" t="s">
         <v>3207</v>
       </c>
       <c r="R16" s="18" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="S16" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="T16" s="37">
-        <f>K16/12.5</f>
-        <v>12</v>
+      <c r="T16" s="36">
+        <f>K16/1</f>
+        <v>11</v>
       </c>
       <c r="U16" s="34">
-        <f>N16-T16</f>
-        <v>0</v>
+        <f t="shared" si="18"/>
+        <v>1</v>
       </c>
       <c r="V16" s="8">
         <v>5</v>
       </c>
       <c r="W16" s="9" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="X16" s="9"/>
       <c r="Y16" s="9"/>
@@ -12921,84 +12883,84 @@
       <c r="AG16" s="9"/>
       <c r="AH16" s="9"/>
       <c r="AI16" s="16" t="b">
-        <f>AND(AJ16:AV16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ16" s="16" t="b">
-        <f>I16=V16</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK16" s="16" t="b">
-        <f>J16=W16</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL16" s="16" t="b">
-        <f>K16=X16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM16" s="16" t="b">
-        <f>L16=Y16</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN16" s="16" t="b">
-        <f>M16=Z16</f>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="AO16" s="16" t="b">
-        <f>N16=AA16</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP16" s="16" t="b">
-        <f>O16=AB16</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ16" s="16" t="b">
-        <f>P16=AC16</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR16" s="16" t="b">
-        <f>Q16=AD16</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS16" s="16" t="b">
-        <f>R16=AE16</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT16" s="16" t="b">
-        <f>S16=AF16</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU16" s="16" t="b">
-        <f>T16=AG16</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV16" s="16" t="b">
-        <f>U16=AH16</f>
-        <v>1</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="AW16" s="16" t="s">
-        <v>3232</v>
+        <v>3246</v>
       </c>
       <c r="AX16" s="16" t="s">
-        <v>3273</v>
+        <v>3280</v>
       </c>
       <c r="AY16" s="16" t="s">
-        <v>3231</v>
+        <v>3245</v>
       </c>
     </row>
     <row r="17" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
-        <f>A16+1</f>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="B17" s="6">
         <v>5</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="22">
-        <v>144</v>
+        <v>74</v>
+      </c>
+      <c r="D17" s="17">
+        <v>120</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
@@ -13007,57 +12969,53 @@
         <v>3214</v>
       </c>
       <c r="I17" s="17">
-        <f>IF(B17="",1,B17)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J17" s="17" t="str">
-        <f>IF(C17="",1,C17)</f>
-        <v>dopamine</v>
+        <f t="shared" si="16"/>
+        <v>labetalol</v>
       </c>
       <c r="K17" s="17">
-        <f>IF(D17="",1.44,D17)</f>
-        <v>144</v>
+        <v>60</v>
       </c>
       <c r="L17" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="M17" s="17" t="str">
-        <f>IF(E17="","glucose 10%",E17)</f>
-        <v>glucose 10%</v>
-      </c>
+      <c r="M17" s="17"/>
       <c r="N17" s="17">
         <f>IF(F17="",12,F17)</f>
         <v>12</v>
       </c>
       <c r="O17" s="20">
-        <f>IF(G17="",0.5,G17)</f>
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="P17" s="32">
-        <v>20</v>
+      <c r="P17" s="31">
+        <v>0.5</v>
       </c>
       <c r="Q17" s="18" t="s">
-        <v>3207</v>
+        <v>3210</v>
       </c>
       <c r="R17" s="18" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="S17" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="T17" s="37">
-        <f>K17/40</f>
-        <v>3.6</v>
+      <c r="T17" s="36">
+        <f>K17/5</f>
+        <v>12</v>
       </c>
       <c r="U17" s="34">
-        <f>N17-T17</f>
-        <v>8.4</v>
+        <f t="shared" si="18"/>
+        <v>0</v>
       </c>
       <c r="V17" s="8">
         <v>5</v>
       </c>
       <c r="W17" s="9" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
@@ -13071,84 +13029,84 @@
       <c r="AG17" s="9"/>
       <c r="AH17" s="9"/>
       <c r="AI17" s="16" t="b">
-        <f>AND(AJ17:AV17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ17" s="16" t="b">
-        <f>I17=V17</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK17" s="16" t="b">
-        <f>J17=W17</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL17" s="16" t="b">
-        <f>K17=X17</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM17" s="16" t="b">
-        <f>L17=Y17</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN17" s="16" t="b">
-        <f>M17=Z17</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="AO17" s="16" t="b">
-        <f>N17=AA17</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP17" s="16" t="b">
-        <f>O17=AB17</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ17" s="16" t="b">
-        <f>P17=AC17</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR17" s="16" t="b">
-        <f>Q17=AD17</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS17" s="16" t="b">
-        <f>R17=AE17</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT17" s="16" t="b">
-        <f>S17=AF17</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU17" s="16" t="b">
-        <f>T17=AG17</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV17" s="16" t="b">
-        <f>U17=AH17</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="AW17" s="16" t="s">
-        <v>3234</v>
+        <v>3248</v>
       </c>
       <c r="AX17" s="16" t="s">
-        <v>3274</v>
+        <v>3281</v>
       </c>
       <c r="AY17" s="16" t="s">
-        <v>3233</v>
+        <v>3247</v>
       </c>
     </row>
     <row r="18" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
-        <f>A17+1</f>
+        <f t="shared" si="14"/>
         <v>16</v>
       </c>
       <c r="B18" s="6">
         <v>5</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D18" s="17">
-        <v>20</v>
+        <v>840</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
@@ -13157,16 +13115,15 @@
         <v>3214</v>
       </c>
       <c r="I18" s="17">
-        <f>IF(B18="",1,B18)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J18" s="17" t="str">
-        <f>IF(C18="",1,C18)</f>
-        <v>furosemide</v>
+        <f t="shared" si="16"/>
+        <v>lidocaine</v>
       </c>
       <c r="K18" s="17">
-        <f>IF(D18="",1.2,D18)</f>
-        <v>20</v>
+        <v>840</v>
       </c>
       <c r="L18" s="18" t="s">
         <v>33</v>
@@ -13176,38 +13133,38 @@
         <v>glucose 10%</v>
       </c>
       <c r="N18" s="17">
-        <f>IF(F18="",12,F18)</f>
-        <v>12</v>
+        <f>IF(F18="",48,F18)</f>
+        <v>48</v>
       </c>
       <c r="O18" s="20">
-        <f>IF(G18="",0.5,G18)</f>
-        <v>0.5</v>
-      </c>
-      <c r="P18" s="32">
-        <v>4</v>
+        <f>IF(G18="",2,G18)</f>
+        <v>2</v>
+      </c>
+      <c r="P18" s="31">
+        <v>7</v>
       </c>
       <c r="Q18" s="18" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
       <c r="R18" s="18" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="S18" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="T18" s="37">
-        <f>K18/10</f>
-        <v>2</v>
+      <c r="T18" s="36">
+        <f>K18/20</f>
+        <v>42</v>
       </c>
       <c r="U18" s="34">
-        <f>N18-T18</f>
-        <v>10</v>
+        <f t="shared" si="18"/>
+        <v>6</v>
       </c>
       <c r="V18" s="8">
         <v>5</v>
       </c>
       <c r="W18" s="9" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="X18" s="9"/>
       <c r="Y18" s="9"/>
@@ -13221,84 +13178,84 @@
       <c r="AG18" s="9"/>
       <c r="AH18" s="9"/>
       <c r="AI18" s="16" t="b">
-        <f>AND(AJ18:AV18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ18" s="16" t="b">
-        <f>I18=V18</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK18" s="16" t="b">
-        <f>J18=W18</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL18" s="16" t="b">
-        <f>K18=X18</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM18" s="16" t="b">
-        <f>L18=Y18</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN18" s="16" t="b">
-        <f>M18=Z18</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AO18" s="16" t="b">
-        <f>N18=AA18</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP18" s="16" t="b">
-        <f>O18=AB18</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ18" s="16" t="b">
-        <f>P18=AC18</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR18" s="16" t="b">
-        <f>Q18=AD18</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS18" s="16" t="b">
-        <f>R18=AE18</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT18" s="16" t="b">
-        <f>S18=AF18</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU18" s="16" t="b">
-        <f>T18=AG18</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV18" s="16" t="b">
-        <f>U18=AH18</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AW18" s="16" t="s">
-        <v>3242</v>
+        <v>3250</v>
       </c>
       <c r="AX18" s="16" t="s">
-        <v>3278</v>
+        <v>3282</v>
       </c>
       <c r="AY18" s="16" t="s">
-        <v>3241</v>
+        <v>3249</v>
       </c>
     </row>
     <row r="19" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
-        <f>A18+1</f>
+        <f t="shared" si="14"/>
         <v>17</v>
       </c>
       <c r="B19" s="6">
         <v>5</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D19" s="17">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
@@ -13307,54 +13264,54 @@
         <v>3214</v>
       </c>
       <c r="I19" s="17">
-        <f>IF(B19="",1,B19)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J19" s="17" t="str">
-        <f>IF(C19="",1,C19)</f>
-        <v>insuline</v>
+        <f t="shared" si="16"/>
+        <v>midazolam</v>
       </c>
       <c r="K19" s="17">
-        <f>IF(D19="",0.24,D19)</f>
-        <v>12</v>
+        <f>IF(D19="",1.2,D19)</f>
+        <v>60</v>
       </c>
       <c r="L19" s="18" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="M19" s="17"/>
       <c r="N19" s="17">
-        <f>IF(F19="",12,F19)</f>
+        <f t="shared" ref="N19:N25" si="19">IF(F19="",12,F19)</f>
         <v>12</v>
       </c>
       <c r="O19" s="20">
-        <f>IF(G19="",0.5,G19)</f>
+        <f t="shared" ref="O19:O25" si="20">IF(G19="",0.5,G19)</f>
         <v>0.5</v>
       </c>
-      <c r="P19" s="32">
-        <v>0.1</v>
+      <c r="P19" s="31">
+        <v>0.5</v>
       </c>
       <c r="Q19" s="18" t="s">
-        <v>3213</v>
+        <v>3210</v>
       </c>
       <c r="R19" s="18" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="S19" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="T19" s="37">
-        <f>K19/1</f>
+      <c r="T19" s="36">
+        <f>K19/5</f>
         <v>12</v>
       </c>
       <c r="U19" s="34">
-        <f>N19-T19</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="V19" s="8">
         <v>5</v>
       </c>
       <c r="W19" s="9" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="X19" s="9"/>
       <c r="Y19" s="9"/>
@@ -13368,84 +13325,84 @@
       <c r="AG19" s="9"/>
       <c r="AH19" s="9"/>
       <c r="AI19" s="16" t="b">
-        <f>AND(AJ19:AV19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ19" s="16" t="b">
-        <f>I19=V19</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK19" s="16" t="b">
-        <f>J19=W19</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL19" s="16" t="b">
-        <f>K19=X19</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM19" s="16" t="b">
-        <f>L19=Y19</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN19" s="16" t="b">
-        <f>M19=Z19</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AO19" s="16" t="b">
-        <f>N19=AA19</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP19" s="16" t="b">
-        <f>O19=AB19</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ19" s="16" t="b">
-        <f>P19=AC19</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR19" s="16" t="b">
-        <f>Q19=AD19</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS19" s="16" t="b">
-        <f>R19=AE19</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT19" s="16" t="b">
-        <f>S19=AF19</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU19" s="16" t="b">
-        <f>T19=AG19</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV19" s="16" t="b">
-        <f>U19=AH19</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AW19" s="16" t="s">
-        <v>3244</v>
+        <v>3252</v>
       </c>
       <c r="AX19" s="16" t="s">
-        <v>3279</v>
+        <v>3283</v>
       </c>
       <c r="AY19" s="16" t="s">
-        <v>3243</v>
+        <v>3251</v>
       </c>
     </row>
     <row r="20" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
-        <f>A19+1</f>
+        <f t="shared" si="14"/>
         <v>18</v>
       </c>
       <c r="B20" s="6">
         <v>5</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D20" s="17">
-        <v>10.8</v>
+        <v>5.4</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
@@ -13454,15 +13411,16 @@
         <v>3214</v>
       </c>
       <c r="I20" s="17">
-        <f>IF(B20="",1,B20)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J20" s="17" t="str">
-        <f>IF(C20="",1,C20)</f>
-        <v>isoprenaline</v>
+        <f t="shared" si="16"/>
+        <v>milrinone</v>
       </c>
       <c r="K20" s="17">
-        <v>11</v>
+        <f>IF(D20="",0.36,D20)</f>
+        <v>5.4</v>
       </c>
       <c r="L20" s="18" t="s">
         <v>33</v>
@@ -13472,38 +13430,38 @@
         <v>glucose 10%</v>
       </c>
       <c r="N20" s="17">
-        <f>IF(F20="",12,F20)</f>
+        <f t="shared" si="19"/>
         <v>12</v>
       </c>
       <c r="O20" s="20">
-        <f>IF(G20="",0.5,G20)</f>
+        <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="P20" s="32">
-        <v>1.5</v>
+      <c r="P20" s="31">
+        <v>0.75</v>
       </c>
       <c r="Q20" s="18" t="s">
         <v>3207</v>
       </c>
       <c r="R20" s="18" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="S20" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="T20" s="37">
+      <c r="T20" s="36">
         <f>K20/1</f>
-        <v>11</v>
+        <v>5.4</v>
       </c>
       <c r="U20" s="34">
-        <f>N20-T20</f>
-        <v>1</v>
+        <f t="shared" si="18"/>
+        <v>6.6</v>
       </c>
       <c r="V20" s="8">
         <v>5</v>
       </c>
       <c r="W20" s="9" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="X20" s="9"/>
       <c r="Y20" s="9"/>
@@ -13517,84 +13475,84 @@
       <c r="AG20" s="9"/>
       <c r="AH20" s="9"/>
       <c r="AI20" s="16" t="b">
-        <f>AND(AJ20:AV20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ20" s="16" t="b">
-        <f>I20=V20</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK20" s="16" t="b">
-        <f>J20=W20</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL20" s="16" t="b">
-        <f>K20=X20</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM20" s="16" t="b">
-        <f>L20=Y20</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN20" s="16" t="b">
-        <f>M20=Z20</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AO20" s="16" t="b">
-        <f>N20=AA20</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP20" s="16" t="b">
-        <f>O20=AB20</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ20" s="16" t="b">
-        <f>P20=AC20</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR20" s="16" t="b">
-        <f>Q20=AD20</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS20" s="16" t="b">
-        <f>R20=AE20</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT20" s="16" t="b">
-        <f>S20=AF20</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU20" s="16" t="b">
-        <f>T20=AG20</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV20" s="16" t="b">
-        <f>U20=AH20</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AW20" s="16" t="s">
-        <v>3246</v>
+        <v>3254</v>
       </c>
       <c r="AX20" s="16" t="s">
-        <v>3280</v>
+        <v>3284</v>
       </c>
       <c r="AY20" s="16" t="s">
-        <v>3245</v>
+        <v>3253</v>
       </c>
     </row>
     <row r="21" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
-        <f>A20+1</f>
+        <f t="shared" si="14"/>
         <v>19</v>
       </c>
       <c r="B21" s="6">
         <v>5</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D21" s="17">
-        <v>840</v>
+        <v>2.5</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
@@ -13603,15 +13561,16 @@
         <v>3214</v>
       </c>
       <c r="I21" s="17">
-        <f>IF(B21="",1,B21)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J21" s="17" t="str">
-        <f>IF(C21="",1,C21)</f>
-        <v>lidocaine</v>
+        <f t="shared" si="16"/>
+        <v>morfine</v>
       </c>
       <c r="K21" s="17">
-        <v>840</v>
+        <f>IF(D21="",0.125,D21)</f>
+        <v>2.5</v>
       </c>
       <c r="L21" s="18" t="s">
         <v>33</v>
@@ -13621,38 +13580,38 @@
         <v>glucose 10%</v>
       </c>
       <c r="N21" s="17">
-        <f>IF(F21="",48,F21)</f>
-        <v>48</v>
+        <f t="shared" si="19"/>
+        <v>12</v>
       </c>
       <c r="O21" s="20">
-        <f>IF(G21="",2,G21)</f>
-        <v>2</v>
-      </c>
-      <c r="P21" s="32">
-        <v>7</v>
+        <f t="shared" si="20"/>
+        <v>0.5</v>
+      </c>
+      <c r="P21" s="31">
+        <v>0.5</v>
       </c>
       <c r="Q21" s="18" t="s">
-        <v>3210</v>
+        <v>3212</v>
       </c>
       <c r="R21" s="18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="S21" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="T21" s="37">
-        <f>K21/20</f>
-        <v>42</v>
+      <c r="T21" s="36">
+        <f>K21/1</f>
+        <v>2.5</v>
       </c>
       <c r="U21" s="34">
-        <f>N21-T21</f>
-        <v>6</v>
+        <f t="shared" si="18"/>
+        <v>9.5</v>
       </c>
       <c r="V21" s="8">
         <v>5</v>
       </c>
       <c r="W21" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="X21" s="9"/>
       <c r="Y21" s="9"/>
@@ -13666,140 +13625,141 @@
       <c r="AG21" s="9"/>
       <c r="AH21" s="9"/>
       <c r="AI21" s="16" t="b">
-        <f>AND(AJ21:AV21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ21" s="16" t="b">
-        <f>I21=V21</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK21" s="16" t="b">
-        <f>J21=W21</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL21" s="16" t="b">
-        <f>K21=X21</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM21" s="16" t="b">
-        <f>L21=Y21</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN21" s="16" t="b">
-        <f>M21=Z21</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AO21" s="16" t="b">
-        <f>N21=AA21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP21" s="16" t="b">
-        <f>O21=AB21</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ21" s="16" t="b">
-        <f>P21=AC21</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR21" s="16" t="b">
-        <f>Q21=AD21</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS21" s="16" t="b">
-        <f>R21=AE21</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT21" s="16" t="b">
-        <f>S21=AF21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU21" s="16" t="b">
-        <f>T21=AG21</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV21" s="16" t="b">
-        <f>U21=AH21</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AW21" s="16" t="s">
-        <v>3250</v>
+        <v>3256</v>
       </c>
       <c r="AX21" s="16" t="s">
-        <v>3282</v>
+        <v>3285</v>
       </c>
       <c r="AY21" s="16" t="s">
-        <v>3249</v>
+        <v>3255</v>
       </c>
     </row>
     <row r="22" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
-        <f>A21+1</f>
+        <f t="shared" si="14"/>
         <v>20</v>
       </c>
       <c r="B22" s="6">
         <v>5</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D22" s="17">
-        <v>60</v>
+        <v>14.4</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
+      <c r="G22" s="17">
+        <v>0.6</v>
+      </c>
       <c r="H22" s="26" t="s">
         <v>3214</v>
       </c>
       <c r="I22" s="17">
-        <f>IF(B22="",1,B22)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J22" s="17" t="str">
-        <f>IF(C22="",1,C22)</f>
-        <v>midazolam</v>
+        <f t="shared" si="16"/>
+        <v>nicardipine</v>
       </c>
       <c r="K22" s="17">
-        <f>IF(D22="",1.2,D22)</f>
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="L22" s="18" t="s">
         <v>33</v>
       </c>
       <c r="M22" s="17"/>
       <c r="N22" s="17">
-        <f>IF(F22="",12,F22)</f>
+        <f t="shared" si="19"/>
         <v>12</v>
       </c>
       <c r="O22" s="20">
-        <f>IF(G22="",0.5,G22)</f>
-        <v>0.5</v>
-      </c>
-      <c r="P22" s="32">
-        <v>0.5</v>
+        <f t="shared" si="20"/>
+        <v>0.6</v>
+      </c>
+      <c r="P22" s="31">
+        <v>2</v>
       </c>
       <c r="Q22" s="18" t="s">
-        <v>3210</v>
+        <v>3207</v>
       </c>
       <c r="R22" s="18" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="S22" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="T22" s="37">
-        <f>K22/5</f>
+        <v>3295</v>
+      </c>
+      <c r="T22" s="36">
+        <f>K22/1</f>
         <v>12</v>
       </c>
       <c r="U22" s="34">
-        <f>N22-T22</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="V22" s="8">
         <v>5</v>
       </c>
       <c r="W22" s="9" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="X22" s="9"/>
       <c r="Y22" s="9"/>
@@ -13813,84 +13773,84 @@
       <c r="AG22" s="9"/>
       <c r="AH22" s="9"/>
       <c r="AI22" s="16" t="b">
-        <f>AND(AJ22:AV22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ22" s="16" t="b">
-        <f>I22=V22</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK22" s="16" t="b">
-        <f>J22=W22</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL22" s="16" t="b">
-        <f>K22=X22</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM22" s="16" t="b">
-        <f>L22=Y22</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN22" s="16" t="b">
-        <f>M22=Z22</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AO22" s="16" t="b">
-        <f>N22=AA22</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP22" s="16" t="b">
-        <f>O22=AB22</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ22" s="16" t="b">
-        <f>P22=AC22</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR22" s="16" t="b">
-        <f>Q22=AD22</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS22" s="16" t="b">
-        <f>R22=AE22</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT22" s="16" t="b">
-        <f>S22=AF22</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU22" s="16" t="b">
-        <f>T22=AG22</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV22" s="16" t="b">
-        <f>U22=AH22</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AW22" s="16" t="s">
-        <v>3252</v>
+        <v>3258</v>
       </c>
       <c r="AX22" s="16" t="s">
-        <v>3283</v>
+        <v>3286</v>
       </c>
       <c r="AY22" s="16" t="s">
-        <v>3251</v>
+        <v>3257</v>
       </c>
     </row>
     <row r="23" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
-        <f>A22+1</f>
+        <f t="shared" si="14"/>
         <v>21</v>
       </c>
       <c r="B23" s="6">
         <v>5</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D23" s="17">
-        <v>5.4</v>
+        <v>57.6</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
@@ -13899,16 +13859,15 @@
         <v>3214</v>
       </c>
       <c r="I23" s="17">
-        <f>IF(B23="",1,B23)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J23" s="17" t="str">
-        <f>IF(C23="",1,C23)</f>
-        <v>milrinone</v>
+        <f t="shared" si="16"/>
+        <v>nitroprusside</v>
       </c>
       <c r="K23" s="17">
-        <f>IF(D23="",0.36,D23)</f>
-        <v>5.4</v>
+        <v>58</v>
       </c>
       <c r="L23" s="18" t="s">
         <v>33</v>
@@ -13918,38 +13877,38 @@
         <v>glucose 10%</v>
       </c>
       <c r="N23" s="17">
-        <f>IF(F23="",12,F23)</f>
+        <f t="shared" si="19"/>
         <v>12</v>
       </c>
       <c r="O23" s="20">
-        <f>IF(G23="",0.5,G23)</f>
+        <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="P23" s="32">
-        <v>0.75</v>
+      <c r="P23" s="31">
+        <v>8.1</v>
       </c>
       <c r="Q23" s="18" t="s">
         <v>3207</v>
       </c>
       <c r="R23" s="18" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="S23" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="T23" s="37">
-        <f>K23/1</f>
-        <v>5.4</v>
+      <c r="T23" s="36">
+        <f>K23/10</f>
+        <v>5.8</v>
       </c>
       <c r="U23" s="34">
-        <f>N23-T23</f>
-        <v>6.6</v>
+        <f t="shared" si="18"/>
+        <v>6.2</v>
       </c>
       <c r="V23" s="8">
         <v>5</v>
       </c>
       <c r="W23" s="9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="X23" s="9"/>
       <c r="Y23" s="9"/>
@@ -13963,143 +13922,141 @@
       <c r="AG23" s="9"/>
       <c r="AH23" s="9"/>
       <c r="AI23" s="16" t="b">
-        <f>AND(AJ23:AV23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ23" s="16" t="b">
-        <f>I23=V23</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK23" s="16" t="b">
-        <f>J23=W23</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL23" s="16" t="b">
-        <f>K23=X23</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM23" s="16" t="b">
-        <f>L23=Y23</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN23" s="16" t="b">
-        <f>M23=Z23</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AO23" s="16" t="b">
-        <f>N23=AA23</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP23" s="16" t="b">
-        <f>O23=AB23</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ23" s="16" t="b">
-        <f>P23=AC23</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR23" s="16" t="b">
-        <f>Q23=AD23</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS23" s="16" t="b">
-        <f>R23=AE23</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT23" s="16" t="b">
-        <f>S23=AF23</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU23" s="16" t="b">
-        <f>T23=AG23</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV23" s="16" t="b">
-        <f>U23=AH23</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AW23" s="16" t="s">
-        <v>3254</v>
+        <v>3260</v>
       </c>
       <c r="AX23" s="16" t="s">
-        <v>3284</v>
+        <v>3287</v>
       </c>
       <c r="AY23" s="16" t="s">
-        <v>3253</v>
+        <v>3259</v>
       </c>
     </row>
     <row r="24" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
-        <f>A23+1</f>
+        <f t="shared" si="14"/>
         <v>22</v>
       </c>
       <c r="B24" s="6">
         <v>5</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D24" s="17">
-        <v>2.5</v>
+        <v>14.4</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
+      <c r="G24" s="17">
+        <v>0.6</v>
+      </c>
       <c r="H24" s="26" t="s">
         <v>3214</v>
       </c>
       <c r="I24" s="17">
-        <f>IF(B24="",1,B24)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J24" s="17" t="str">
-        <f>IF(C24="",1,C24)</f>
-        <v>morfine</v>
+        <f t="shared" si="16"/>
+        <v>noradrenaline</v>
       </c>
       <c r="K24" s="17">
-        <f>IF(D24="",0.125,D24)</f>
-        <v>2.5</v>
+        <v>12</v>
       </c>
       <c r="L24" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="M24" s="17" t="str">
-        <f>IF(E24="","glucose 10%",E24)</f>
-        <v>glucose 10%</v>
-      </c>
+      <c r="M24" s="17"/>
       <c r="N24" s="17">
-        <f>IF(F24="",12,F24)</f>
+        <f t="shared" si="19"/>
         <v>12</v>
       </c>
       <c r="O24" s="20">
-        <f>IF(G24="",0.5,G24)</f>
-        <v>0.5</v>
-      </c>
-      <c r="P24" s="32">
-        <v>0.5</v>
+        <f t="shared" si="20"/>
+        <v>0.6</v>
+      </c>
+      <c r="P24" s="31">
+        <v>2</v>
       </c>
       <c r="Q24" s="18" t="s">
-        <v>3212</v>
+        <v>3207</v>
       </c>
       <c r="R24" s="18" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="S24" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="T24" s="37">
+        <v>3295</v>
+      </c>
+      <c r="T24" s="36">
         <f>K24/1</f>
-        <v>2.5</v>
+        <v>12</v>
       </c>
       <c r="U24" s="34">
-        <f>N24-T24</f>
-        <v>9.5</v>
+        <f t="shared" si="18"/>
+        <v>0</v>
       </c>
       <c r="V24" s="8">
         <v>5</v>
       </c>
       <c r="W24" s="9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="X24" s="9"/>
       <c r="Y24" s="9"/>
@@ -14113,84 +14070,84 @@
       <c r="AG24" s="9"/>
       <c r="AH24" s="9"/>
       <c r="AI24" s="16" t="b">
-        <f>AND(AJ24:AV24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ24" s="16" t="b">
-        <f>I24=V24</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK24" s="16" t="b">
-        <f>J24=W24</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL24" s="16" t="b">
-        <f>K24=X24</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM24" s="16" t="b">
-        <f>L24=Y24</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN24" s="16" t="b">
-        <f>M24=Z24</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="AO24" s="16" t="b">
-        <f>N24=AA24</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP24" s="16" t="b">
-        <f>O24=AB24</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ24" s="16" t="b">
-        <f>P24=AC24</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR24" s="16" t="b">
-        <f>Q24=AD24</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS24" s="16" t="b">
-        <f>R24=AE24</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT24" s="16" t="b">
-        <f>S24=AF24</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU24" s="16" t="b">
-        <f>T24=AG24</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV24" s="16" t="b">
-        <f>U24=AH24</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="AW24" s="16" t="s">
-        <v>3256</v>
+        <v>3262</v>
       </c>
       <c r="AX24" s="16" t="s">
-        <v>3285</v>
+        <v>3288</v>
       </c>
       <c r="AY24" s="16" t="s">
-        <v>3255</v>
+        <v>3261</v>
       </c>
     </row>
     <row r="25" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
-        <f>A24+1</f>
+        <f t="shared" si="14"/>
         <v>23</v>
       </c>
       <c r="B25" s="6">
         <v>5</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D25" s="17">
-        <v>57.6</v>
+        <v>240</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
@@ -14199,56 +14156,53 @@
         <v>3214</v>
       </c>
       <c r="I25" s="17">
-        <f>IF(B25="",1,B25)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J25" s="17" t="str">
-        <f>IF(C25="",1,C25)</f>
-        <v>nitroprusside</v>
+        <f t="shared" si="16"/>
+        <v>rocuronium</v>
       </c>
       <c r="K25" s="17">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="L25" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="M25" s="17" t="str">
-        <f>IF(E25="","glucose 10%",E25)</f>
-        <v>glucose 10%</v>
-      </c>
+      <c r="M25" s="17"/>
       <c r="N25" s="17">
-        <f>IF(F25="",12,F25)</f>
+        <f t="shared" si="19"/>
         <v>12</v>
       </c>
       <c r="O25" s="20">
-        <f>IF(G25="",0.5,G25)</f>
+        <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
-      <c r="P25" s="32">
-        <v>8.1</v>
+      <c r="P25" s="31">
+        <v>1</v>
       </c>
       <c r="Q25" s="18" t="s">
-        <v>3207</v>
+        <v>3210</v>
       </c>
       <c r="R25" s="18" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="S25" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="T25" s="37">
+      <c r="T25" s="36">
         <f>K25/10</f>
-        <v>5.8</v>
+        <v>12</v>
       </c>
       <c r="U25" s="34">
-        <f>N25-T25</f>
-        <v>6.2</v>
+        <f t="shared" si="18"/>
+        <v>0</v>
       </c>
       <c r="V25" s="8">
         <v>5</v>
       </c>
       <c r="W25" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="X25" s="9"/>
       <c r="Y25" s="9"/>
@@ -14262,74 +14216,74 @@
       <c r="AG25" s="9"/>
       <c r="AH25" s="9"/>
       <c r="AI25" s="16" t="b">
-        <f>AND(AJ25:AV25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ25" s="16" t="b">
-        <f>I25=V25</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK25" s="16" t="b">
-        <f>J25=W25</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL25" s="16" t="b">
-        <f>K25=X25</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM25" s="16" t="b">
-        <f>L25=Y25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN25" s="16" t="b">
-        <f>M25=Z25</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="AO25" s="16" t="b">
-        <f>N25=AA25</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP25" s="16" t="b">
-        <f>O25=AB25</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ25" s="16" t="b">
-        <f>P25=AC25</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR25" s="16" t="b">
-        <f>Q25=AD25</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS25" s="16" t="b">
-        <f>R25=AE25</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT25" s="16" t="b">
-        <f>S25=AF25</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU25" s="16" t="b">
-        <f>T25=AG25</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV25" s="16" t="b">
-        <f>U25=AH25</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="AW25" s="16" t="s">
-        <v>3260</v>
+        <v>3264</v>
       </c>
       <c r="AX25" s="16" t="s">
-        <v>3287</v>
+        <v>3289</v>
       </c>
       <c r="AY25" s="16" t="s">
-        <v>3259</v>
+        <v>3263</v>
       </c>
     </row>
     <row r="26" spans="1:51" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
-        <f>A25+1</f>
+        <f t="shared" si="14"/>
         <v>24</v>
       </c>
       <c r="B26" s="6">
@@ -14348,11 +14302,11 @@
         <v>3214</v>
       </c>
       <c r="I26" s="17">
-        <f>IF(B26="",1,B26)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J26" s="17" t="str">
-        <f>IF(C26="",1,C26)</f>
+        <f t="shared" si="16"/>
         <v>sufentanil/bupivac EPIDURAAL</v>
       </c>
       <c r="K26" s="18">
@@ -14384,7 +14338,7 @@
       <c r="S26" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="T26" s="37">
+      <c r="T26" s="36">
         <f>K26/1</f>
         <v>5</v>
       </c>
@@ -14409,59 +14363,59 @@
       <c r="AG26" s="9"/>
       <c r="AH26" s="9"/>
       <c r="AI26" s="16" t="b">
-        <f>AND(AJ26:AV26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ26" s="16" t="b">
-        <f>I26=V26</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AK26" s="16" t="b">
-        <f>J26=W26</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL26" s="16" t="b">
-        <f>K26=X26</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM26" s="16" t="b">
-        <f>L26=Y26</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN26" s="16" t="b">
-        <f>M26=Z26</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AO26" s="16" t="b">
-        <f>N26=AA26</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP26" s="16" t="b">
-        <f>O26=AB26</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ26" s="16" t="b">
-        <f>P26=AC26</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR26" s="16" t="b">
-        <f>Q26=AD26</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AS26" s="16" t="b">
-        <f>R26=AE26</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT26" s="16" t="b">
-        <f>S26=AF26</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AU26" s="16" t="b">
-        <f>T26=AG26</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV26" s="16" t="b">
-        <f>U26=AH26</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AW26" s="16" t="s">
@@ -14479,65 +14433,65 @@
         <v>20</v>
       </c>
       <c r="AI27" s="16" t="b">
-        <f>AND(AI3:AI26)</f>
+        <f t="shared" ref="AI27:AV27" si="21">AND(AI4:AI26)</f>
         <v>0</v>
       </c>
       <c r="AJ27" s="16" t="b">
-        <f>AND(AJ3:AJ26)</f>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="AK27" s="16" t="b">
-        <f>AND(AK3:AK26)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AL27" s="16" t="b">
-        <f>AND(AL3:AL26)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AM27" s="16" t="b">
-        <f>AND(AM3:AM26)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AN27" s="16" t="b">
-        <f>AND(AN3:AN26)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AO27" s="16" t="b">
-        <f>AND(AO3:AO26)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AP27" s="16" t="b">
-        <f>AND(AP3:AP26)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ27" s="16" t="b">
-        <f>AND(AQ3:AQ26)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AR27" s="16" t="b">
-        <f>AND(AR3:AR26)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AS27" s="16" t="b">
-        <f>AND(AS3:AS26)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AT27" s="16" t="b">
-        <f>AND(AT3:AT26)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AU27" s="16" t="b">
-        <f>AND(AU3:AU26)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AV27" s="16" t="b">
-        <f>AND(AV3:AV26)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection password="CC20" sheet="1" objects="1" scenarios="1"/>
-  <conditionalFormatting sqref="AI3:AV4 AI6:AV26">
+  <conditionalFormatting sqref="AI7:AV26 AI3:AV5">
     <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -14553,7 +14507,7 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI5:AV5">
+  <conditionalFormatting sqref="AI6:AV6">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>

</xml_diff>